<commit_message>
Updated BOM with Screws
</commit_message>
<xml_diff>
--- a/F1TENTH - Bill of Materials Deutschland: Germany: EU/Master BOM Germany.xlsx
+++ b/F1TENTH - Bill of Materials Deutschland: Germany: EU/Master BOM Germany.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tumde.sharepoint.com/sites/AFS/Shared Documents/04_Projects/06_F1TENTH/Bill of Materials - Germany/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjahncke/Desktop/F1TENTH_Auxiliaries/F1TENTH - Bill of Materials Deutschland: Germany: EU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="8_{96579189-E236-1346-90FB-E7C629B7C6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73F4A012-65E8-3F49-B875-33303BE92C18}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0D8F6B-72C4-8648-A7C3-A438E46AAB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="-4760" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slash + Orin Nano" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>Scroll right to see links</t>
   </si>
@@ -178,15 +178,6 @@
     <t>https://www.conrad.de/de/p/absima-1-10-1-8-montagestaender-schwarz-1537809.html</t>
   </si>
   <si>
-    <t>standoff M3 SW6 45mm</t>
-  </si>
-  <si>
-    <t>standoff M3 SW6 25mm</t>
-  </si>
-  <si>
-    <t>standoff M3 SW6 20mm</t>
-  </si>
-  <si>
     <t>https://abstandsbolzen-shop.de/abstandsbolzen/stahl/innen-innengewinde/16/stahl-abstandsbolzen-i/i-gewinde-m3-sw-6?number=BM345&amp;c=15</t>
   </si>
   <si>
@@ -196,9 +187,6 @@
     <t>https://abstandsbolzen-shop.de/abstandsbolzen/stahl/innen-innengewinde/16/stahl-abstandsbolzen-i/i-gewinde-m3-sw-6?number=BM325&amp;c=15</t>
   </si>
   <si>
-    <t>pack of 100</t>
-  </si>
-  <si>
     <t>USB A to USB micro cable</t>
   </si>
   <si>
@@ -235,9 +223,6 @@
     <t>Shrink tube for Servo cable</t>
   </si>
   <si>
-    <t>https://www.conrad.de/de/p/toolland-has07-schrumpfschlauchsortiment-schwarz-1-set-2574855.html#productDescription</t>
-  </si>
-  <si>
     <t>PPM cable for VESC 6</t>
   </si>
   <si>
@@ -257,6 +242,74 @@
   </si>
   <si>
     <t>all prices incl. 19% German federal tax</t>
+  </si>
+  <si>
+    <t>Standoff M3 SW6 45mm</t>
+  </si>
+  <si>
+    <t>Standoff M3 SW6 25mm</t>
+  </si>
+  <si>
+    <t>Standoff M3 SW6 20mm</t>
+  </si>
+  <si>
+    <t>Screws M3x14mm</t>
+  </si>
+  <si>
+    <t>Screws M3x8mm</t>
+  </si>
+  <si>
+    <t>pack of 100
+for Jetson</t>
+  </si>
+  <si>
+    <t>pack of 100
+for Powerboard</t>
+  </si>
+  <si>
+    <t>pack of 100
+for Autonomy Platform</t>
+  </si>
+  <si>
+    <t>Screws M3x20mm</t>
+  </si>
+  <si>
+    <t>Screws M5x</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/p/toolcraft-888123-zylinderschrauben-m3-8-mm-sechsrund-iso-14579-stahl-verzinkt-100-st-888123.html?refresh=true</t>
+  </si>
+  <si>
+    <t>pack of 100
+2x for LiDAR-Camera mount</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/p/iso4017-din933-m3x20-sechskantschraube-gewinde-bis-kopf-vollgewinde-material-a2-blank-100-stueck-865407903.html</t>
+  </si>
+  <si>
+    <t>pack of 100
+4x for Jetson top
+3x for Powerboard op
+2x for ZED 2</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/p/iso4762-din912-m3x14-zylinderschrauben-mit-innensechskant-vollgewinde-material-a2-blank-100-stueck-865439039.html</t>
+  </si>
+  <si>
+    <t>pack of 100
+3x for Autonomy Platform
+4x for Jetson bottom
+3x for Powerboard bottom</t>
+  </si>
+  <si>
+    <t>pack of 100
+2x for VESC</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/p/zylinderschraube-din-912-innen-6kt-m5x20-8-8-galv-verz-100st-806478117.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.conrad.de/de/p/toolland-has07-schrumpfschlauchsortiment-schwarz-1-set-2574855.html#productDescription </t>
   </si>
 </sst>
 </file>
@@ -264,7 +317,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -401,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -421,117 +474,87 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -755,7 +778,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F9" sqref="F9"/>
+      <selection pane="topRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -769,778 +792,830 @@
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-    </row>
-    <row r="3" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="57">
+      <c r="C3" s="10">
         <v>429.95</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48" t="s">
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-    </row>
-    <row r="4" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="57">
+      <c r="C4" s="10">
         <v>249.95</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-    </row>
-    <row r="5" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-    </row>
-    <row r="6" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10">
+        <v>36.51</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="30">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10">
+        <v>21.6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10">
+        <v>21.07</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10">
+        <f>1.8*1.19</f>
+        <v>2.1419999999999999</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10">
+        <f>24.36*1.19</f>
+        <v>28.988399999999999</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10">
+        <f>3.05*1.19</f>
+        <v>3.6294999999999997</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="10">
+        <f>5.35*1.19</f>
+        <v>6.3664999999999994</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="57">
-        <v>36.51</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="29" t="s">
+      <c r="C14" s="10">
+        <v>617.61</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-    </row>
-    <row r="7" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="30">
+      <c r="F14" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C7" s="57">
-        <v>21.6</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-    </row>
-    <row r="8" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="30">
-        <v>1</v>
-      </c>
-      <c r="C8" s="57">
-        <v>21.07</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-    </row>
-    <row r="9" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-    </row>
-    <row r="10" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-    </row>
-    <row r="11" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-    </row>
-    <row r="12" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-    </row>
-    <row r="13" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-    </row>
-    <row r="14" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="30">
-        <v>1</v>
-      </c>
-      <c r="C14" s="57">
-        <v>617.61</v>
-      </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="44"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="54"/>
-      <c r="V14" s="54"/>
-      <c r="W14" s="54"/>
-      <c r="X14" s="54"/>
-      <c r="Y14" s="54"/>
-      <c r="Z14" s="54"/>
-    </row>
-    <row r="15" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="30">
-        <v>1</v>
-      </c>
-      <c r="C15" s="57">
+      <c r="C15" s="10">
         <f>13.44*1.19</f>
         <v>15.993599999999999</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="54"/>
-      <c r="V15" s="54"/>
-      <c r="W15" s="54"/>
-      <c r="X15" s="54"/>
-      <c r="Y15" s="54"/>
-      <c r="Z15" s="54"/>
-      <c r="AA15" s="54"/>
-    </row>
-    <row r="16" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="2">
         <v>1</v>
       </c>
-      <c r="C16" s="57">
+      <c r="C16" s="10">
         <f>82.19*1.19</f>
         <v>97.806099999999986</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44" t="s">
+      <c r="D16" s="22"/>
+      <c r="E16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="54"/>
-      <c r="S16" s="54"/>
-      <c r="T16" s="54"/>
-      <c r="U16" s="54"/>
-      <c r="V16" s="54"/>
-      <c r="W16" s="54"/>
-      <c r="X16" s="54"/>
-      <c r="Y16" s="54"/>
-      <c r="Z16" s="54"/>
-      <c r="AA16" s="54"/>
-    </row>
-    <row r="17" spans="1:27" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+    </row>
+    <row r="17" spans="1:27" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="57">
+      <c r="C17" s="10">
         <f>25.2*1.19</f>
         <v>29.988</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="54"/>
-      <c r="T17" s="54"/>
-      <c r="U17" s="54"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="54"/>
-      <c r="AA17" s="54"/>
-    </row>
-    <row r="18" spans="1:27" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+    </row>
+    <row r="18" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="57">
+      <c r="C18" s="10">
         <f>1.19*12.52</f>
         <v>14.8988</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-    </row>
-    <row r="19" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
-      <c r="AA19" s="13"/>
-    </row>
-    <row r="20" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+    </row>
+    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="10">
         <v>449</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27" t="s">
+      <c r="D20" s="23"/>
+      <c r="E20" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="13"/>
-      <c r="Z20" s="13"/>
-      <c r="AA20" s="13"/>
-    </row>
-    <row r="21" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+    </row>
+    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="10">
         <v>1606.5</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26" t="s">
+      <c r="D21" s="22"/>
+      <c r="E21" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="13"/>
-    </row>
-    <row r="22" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
+      <c r="G21" s="22"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+    </row>
+    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
-    </row>
-    <row r="23" spans="1:27" s="12" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+    </row>
+    <row r="23" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="2">
         <v>1</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="10">
         <v>413.62</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="13"/>
-    </row>
-    <row r="24" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+    </row>
+    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="10">
         <f>64.04*1.19</f>
         <v>76.207599999999999</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="13"/>
-      <c r="Y24" s="13"/>
-      <c r="Z24" s="13"/>
-      <c r="AA24" s="13"/>
-    </row>
-    <row r="25" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="10">
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+    </row>
+    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="10">
         <f>3.35*1.19</f>
         <v>3.9864999999999999</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="9" t="s">
+      <c r="D25" s="26"/>
+      <c r="E25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="13"/>
-    </row>
-    <row r="26" spans="1:27" s="12" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="10">
+      <c r="F25" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+    </row>
+    <row r="26" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="10">
         <v>24.99</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13"/>
-      <c r="AA26" s="13"/>
+      <c r="F26" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
     </row>
     <row r="27" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="30">
+        <v>63</v>
+      </c>
+      <c r="B27" s="2">
         <v>1</v>
       </c>
-      <c r="C27" s="60">
+      <c r="C27" s="1">
         <v>7.98</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="15" t="s">
-        <v>69</v>
+      <c r="F27" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1548,374 +1623,374 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:27" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="10">
+    <row r="28" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="10">
         <f>1.67*1.19</f>
         <v>1.9872999999999998</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11" t="s">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
-      <c r="W28" s="13"/>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
-      <c r="AA28" s="13"/>
-    </row>
-    <row r="29" spans="1:27" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="30">
+      <c r="F28" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+    </row>
+    <row r="29" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="2">
         <v>1</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="10">
         <f>5.84*1.19</f>
         <v>6.9495999999999993</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="29" t="s">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-    </row>
-    <row r="30" spans="1:27" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="10">
+      <c r="F29" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="2">
         <v>1</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="10">
         <v>4.99</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11" t="s">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
-      <c r="U30" s="13"/>
-      <c r="V30" s="13"/>
-      <c r="W30" s="13"/>
-      <c r="X30" s="13"/>
-      <c r="Y30" s="13"/>
-      <c r="Z30" s="13"/>
-      <c r="AA30" s="13"/>
-    </row>
-    <row r="31" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
+      <c r="F30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="9"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
+    </row>
+    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
-      <c r="U31" s="13"/>
-      <c r="V31" s="13"/>
-      <c r="W31" s="13"/>
-      <c r="X31" s="13"/>
-      <c r="Y31" s="13"/>
-      <c r="Z31" s="13"/>
-      <c r="AA31" s="13"/>
-    </row>
-    <row r="32" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+    </row>
+    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="2">
         <v>1</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="10">
         <f>7.55*1.19</f>
         <v>8.9844999999999988</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9" t="s">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13"/>
-      <c r="U32" s="13"/>
-      <c r="V32" s="13"/>
-      <c r="W32" s="13"/>
-      <c r="X32" s="13"/>
-      <c r="Y32" s="13"/>
-      <c r="Z32" s="13"/>
-      <c r="AA32" s="13"/>
-    </row>
-    <row r="33" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
+    </row>
+    <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="2">
         <v>1</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="10">
         <f>1.19*20.97</f>
         <v>24.954299999999996</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26" t="s">
+      <c r="D33" s="22"/>
+      <c r="E33" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F33" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13"/>
-      <c r="U33" s="13"/>
-      <c r="V33" s="13"/>
-      <c r="W33" s="13"/>
-      <c r="X33" s="13"/>
-      <c r="Y33" s="13"/>
-      <c r="Z33" s="13"/>
-      <c r="AA33" s="13"/>
-    </row>
-    <row r="34" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="10">
+      <c r="G33" s="19"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="9"/>
+      <c r="Y33" s="9"/>
+      <c r="Z33" s="9"/>
+      <c r="AA33" s="9"/>
+    </row>
+    <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="2">
         <v>1</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="10">
         <f>7.5*1.19</f>
         <v>8.9249999999999989</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11" t="s">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13"/>
-      <c r="U34" s="13"/>
-      <c r="V34" s="13"/>
-      <c r="W34" s="13"/>
-      <c r="X34" s="13"/>
-      <c r="Y34" s="13"/>
-      <c r="Z34" s="13"/>
-      <c r="AA34" s="13"/>
-    </row>
-    <row r="35" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="10">
+      <c r="F34" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="9"/>
+      <c r="V34" s="9"/>
+      <c r="W34" s="9"/>
+      <c r="X34" s="9"/>
+      <c r="Y34" s="9"/>
+      <c r="Z34" s="9"/>
+      <c r="AA34" s="9"/>
+    </row>
+    <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="2">
         <v>1</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="10">
         <v>29.99</v>
       </c>
-      <c r="D35" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="26" t="s">
+      <c r="D35" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="G35" s="38"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
-      <c r="U35" s="13"/>
-      <c r="V35" s="13"/>
-      <c r="W35" s="13"/>
-      <c r="X35" s="13"/>
-      <c r="Y35" s="13"/>
-      <c r="Z35" s="13"/>
-      <c r="AA35" s="13"/>
-    </row>
-    <row r="36" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="F35" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="10">
+      <c r="G35" s="41"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="9"/>
+      <c r="Y35" s="9"/>
+      <c r="Z35" s="9"/>
+      <c r="AA35" s="9"/>
+    </row>
+    <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="2">
         <v>1</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="10">
         <f>1.67*1.19</f>
         <v>1.9872999999999998</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26" t="s">
+      <c r="D36" s="22"/>
+      <c r="E36" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="G36" s="23"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
-      <c r="W36" s="13"/>
-      <c r="X36" s="13"/>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="13"/>
-    </row>
-    <row r="37" spans="1:27" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-    </row>
-    <row r="38" spans="1:27" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="40"/>
-      <c r="B38" s="41" t="s">
+      <c r="F36" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="19"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="9"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="9"/>
+      <c r="Z36" s="9"/>
+      <c r="AA36" s="9"/>
+    </row>
+    <row r="37" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="61">
+      <c r="C38" s="40">
         <f>SUM(C1:C35)+C32+C12*3</f>
-        <v>4213.4257999999991</v>
-      </c>
-      <c r="D38" s="11" t="s">
+        <v>4273.6516999999985</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
@@ -1949,7 +2024,7 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -5220,12 +5295,36 @@
     <hyperlink ref="F30" r:id="rId14" xr:uid="{E6363950-9D1D-ED48-8856-22ECF842D4BD}"/>
     <hyperlink ref="F27" r:id="rId15" display="https://www.ebay.de/itm/195564348829?hash=item2d888b259d:g:694AAOSwE3ljyaFR&amp;amdata=enc%3AAQAIAAAA8CUtDB%2B13vHLE9fhMNhfwzKAlt%2F0rYczyeexMYnIdTL%2FI3a5l3mOSnrm8WhvG7bOSVYrIw4QYnXwPG4kUTB%2B4qJb03uxgZnADwOO9wSp7zbbRztAe72XaRjjXoLItyPp5bCFKzcHnZ6xHdwDDCwJ6jnrvUTxWAPj9iSIJA%2BoyROS5S1Jv6Si5V0%2Bz%2Fox%2BHcEmYmkU4dkXaVNZIFd%2BOWHghgjFOXC4iI6MNAOXCotNyslUqnc6c4hyyWIrqXb3WD1EH%2Bcw1zCYAWyPdBX%2Br6%2B4B0akaPXlT3Cn2wD8mkNQ0NgiDluCyfrVV9UpyCnSFCNaQ%3D%3D%7Ctkp%3ABk9SR8a49o77Yg" xr:uid="{12DDD26A-B4B3-7F46-9334-0BFD406DB8AB}"/>
     <hyperlink ref="F34" r:id="rId16" location="productDescription" xr:uid="{3B8ED911-F821-F641-A671-D8E9A8B8ECAB}"/>
+    <hyperlink ref="F10" r:id="rId17" xr:uid="{F6A2E5D1-1432-CE4B-B5D9-01400EE80038}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{3A91A690-6290-B84F-BA51-1FFA8C2E3504}"/>
+    <hyperlink ref="F12" r:id="rId19" xr:uid="{9892B74E-3369-2947-B5C1-E1D4FE3359FF}"/>
+    <hyperlink ref="F29" r:id="rId20" location="productDescription " xr:uid="{26D2F4F4-B093-DE48-AF81-90D24070E941}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a73fa131-f58a-4a5f-826b-52579997d9e6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d939e73f-5984-40c2-86cb-067d1ef853e9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A2DBA1DBACA459409CC289C7441DF1DC" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="1c1a65b77858e714f0680482ae9fe8e0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a73fa131-f58a-4a5f-826b-52579997d9e6" xmlns:ns3="d939e73f-5984-40c2-86cb-067d1ef853e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e565aca8b2d012d21ccf9a2cbc87f1b6" ns2:_="" ns3:_="">
     <xsd:import namespace="a73fa131-f58a-4a5f-826b-52579997d9e6"/>
@@ -5448,34 +5547,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a73fa131-f58a-4a5f-826b-52579997d9e6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d939e73f-5984-40c2-86cb-067d1ef853e9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41F0D3FE-60E7-4E66-A7E7-480F6DD044A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{786D5654-74D6-48D6-94DC-CB923F37A1A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a73fa131-f58a-4a5f-826b-52579997d9e6"/>
+    <ds:schemaRef ds:uri="d939e73f-5984-40c2-86cb-067d1ef853e9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E01EBAD9-889A-4467-B78E-9B0D6629F53E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E01EBAD9-889A-4467-B78E-9B0D6629F53E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{786D5654-74D6-48D6-94DC-CB923F37A1A9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41F0D3FE-60E7-4E66-A7E7-480F6DD044A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a73fa131-f58a-4a5f-826b-52579997d9e6"/>
+    <ds:schemaRef ds:uri="d939e73f-5984-40c2-86cb-067d1ef853e9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>